<commit_message>
manage change from prek12plaza to geniusplaza
</commit_message>
<xml_diff>
--- a/PreK12Plaza Learning Objects 2017-01-11.xlsx
+++ b/PreK12Plaza Learning Objects 2017-01-11.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="1st Grade ELA" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,12 @@
     <sheet name="Teacher - Professional Develop" sheetId="43" r:id="rId43"/>
     <sheet name="Teacher - Resources" sheetId="44" r:id="rId44"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -11696,8 +11701,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12030,12 +12035,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="35.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -16939,16 +16947,21 @@
     <hyperlink ref="H183" r:id="rId182"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -20865,16 +20878,21 @@
     <hyperlink ref="H148" r:id="rId147"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -21824,16 +21842,21 @@
     <hyperlink ref="H35" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -21863,16 +21886,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -25282,16 +25310,21 @@
     <hyperlink ref="H131" r:id="rId130"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -25782,16 +25815,21 @@
     <hyperlink ref="H18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -26729,16 +26767,21 @@
     <hyperlink ref="H36" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -26824,16 +26867,21 @@
     <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -27150,16 +27198,21 @@
     <hyperlink ref="H12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -27317,16 +27370,21 @@
     <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -29134,16 +29192,21 @@
     <hyperlink ref="H70" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -29526,16 +29589,21 @@
     <hyperlink ref="H14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -29636,16 +29704,21 @@
     <hyperlink ref="H4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -30718,16 +30791,21 @@
     <hyperlink ref="H41" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -31815,16 +31893,21 @@
     <hyperlink ref="H45" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -33668,16 +33751,21 @@
     <hyperlink ref="H71" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -33757,16 +33845,21 @@
     <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -33796,16 +33889,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -34611,16 +34709,21 @@
     <hyperlink ref="H34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -34650,16 +34753,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -34689,16 +34797,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -35243,16 +35356,21 @@
     <hyperlink ref="H20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -38683,16 +38801,21 @@
     <hyperlink ref="H131" r:id="rId130"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -38748,16 +38871,21 @@
     <hyperlink ref="H2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -38787,16 +38915,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H363"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -48536,16 +48669,21 @@
     <hyperlink ref="H363" r:id="rId362"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49210,16 +49348,21 @@
     <hyperlink ref="H25" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49299,16 +49442,21 @@
     <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49338,16 +49486,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49377,16 +49530,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49416,16 +49574,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -49673,16 +49836,21 @@
     <hyperlink ref="H9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -50113,16 +50281,21 @@
     <hyperlink ref="H16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -50991,16 +51164,21 @@
     <hyperlink ref="H32" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -51030,16 +51208,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -51069,16 +51252,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -51230,16 +51418,21 @@
     <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -51269,16 +51462,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -51308,16 +51506,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -54889,16 +55092,21 @@
     <hyperlink ref="H136" r:id="rId135"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -56172,16 +56380,21 @@
     <hyperlink ref="H47" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -59261,16 +59474,21 @@
     <hyperlink ref="H117" r:id="rId116"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -60913,16 +61131,21 @@
     <hyperlink ref="H61" r:id="rId60"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -60952,5 +61175,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>